<commit_message>
Adding in the JMX normalized table for catch data.
</commit_message>
<xml_diff>
--- a/documents/field-sampling/sample-data-sheets/WDFW_smolt_data_examples/0708 TUCANNON LW.xlsx
+++ b/documents/field-sampling/sample-data-sheets/WDFW_smolt_data_examples/0708 TUCANNON LW.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="11295" windowHeight="6495"/>
+    <workbookView minimized="1" xWindow="40440" yWindow="2820" windowWidth="21820" windowHeight="19060" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Raw Data" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,11 @@
     <sheet name="Week Numbers" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -227,8 +232,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="d\-mmm"/>
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -454,14 +462,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -514,7 +522,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -802,25 +810,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr codeName="Sheet1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" codeName="Sheet1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:K3806"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A359" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12"/>
   <cols>
-    <col min="2" max="2" width="8.85546875" style="18" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" style="9" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" style="16" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" style="18" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" style="9" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" style="16" customWidth="1"/>
     <col min="7" max="7" width="11" style="24" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" style="16" customWidth="1"/>
+    <col min="8" max="8" width="9.83203125" style="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18">
+    <row r="1" spans="1:11" ht="17">
       <c r="A1" s="14" t="s">
         <v>15</v>
       </c>
@@ -43162,22 +43170,28 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A2:J534"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12"/>
   <sheetData>
     <row r="2" spans="1:10">
       <c r="A2" s="7"/>
@@ -56737,15 +56751,21 @@
       <c r="J534" s="37"/>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr codeName="Sheet3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" codeName="Sheet3" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AA1701"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
@@ -56753,7 +56773,7 @@
       <selection pane="bottomLeft" activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12"/>
   <sheetData>
     <row r="1" spans="1:27">
       <c r="A1" s="20"/>
@@ -88553,25 +88573,32 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="B3:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12"/>
   <cols>
-    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:7">
@@ -88869,8 +88896,14 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>